<commit_message>
Refactor document processing and enhance search tools. Migrate document search functionality to a new structure, implement caching for vector store, and add support for Excel file processing. Introduce new API endpoints for cache management and improve error handling across tools. Update dependencies in package.json and package-lock.json.
</commit_message>
<xml_diff>
--- a/data/Chatbot Soruları ve Cevapları.xlsx
+++ b/data/Chatbot Soruları ve Cevapları.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Custom Documents\Projects\Proje Deneme\libchatgemini\back\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Custom Documents\Projects\Proje Deneme\lgraph\data\archive\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6656881-B4C9-4872-A6F3-186A4F243495}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A0EE873-B418-4CC9-A62C-C61357EA5511}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2685" yWindow="2685" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="bu 100 soruyu tek bir sütunda t" sheetId="1" r:id="rId1"/>
@@ -49,29 +49,6 @@
   </si>
   <si>
     <t>27. Scopus veya Web of Science'a nasıl erişebilirim?</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Doğrudan bu </t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="10"/>
-        <color rgb="FF1155CC"/>
-        <rFont val="Arial"/>
-      </rPr>
-      <t>https://kutuphane.itu.edu.tr/arastirma/veritabanlari#harf-A</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> linkten veritabanlarına ulaşıp, bu veritabanları içerisinden Scopus veya Web of Science'a ulaşabilirsiniz. Ya da kütüphane anasayfasındaki "Tarıyorum" arama çubuğun hemen altındaki "veritabanları" linkine tıklıyarak Scopus veya Web of Science'a ulaşabilirsiniz.</t>
-    </r>
   </si>
   <si>
     <t>28. Kampüs dışından veritabanlarına nasıl bağlanabilirim? (Proxy/VPN ayarları)</t>
@@ -869,6 +846,29 @@
   </si>
   <si>
     <t>Kütüphanenin veritabanları sayfasını ziyaret edebilirsiniz: https://kutuphane.itu.edu.tr/arastirma/veritabanlari Sol tarafta bulunan yayın türü bölümünde filtreleme yaparak ilgili veritabanlarını bulabilirsiniz.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Doğrudan bu </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="10"/>
+        <color rgb="FF1155CC"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>https://kutuphane.itu.edu.tr/arastirma/veritabanlari</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> linkten veritabanlarına ulaşıp, bu veritabanları içerisinden Scopus veya Web of Science'a ulaşabilirsiniz. Ya da kütüphane anasayfasındaki "Tarıyorum" arama çubuğun hemen altındaki "veritabanları" linkine tıklıyarak Scopus veya Web of Science'a ulaşabilirsiniz.</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -1199,7 +1199,7 @@
   <dimension ref="A1:Z963"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B34" sqref="B34"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1270,496 +1270,496 @@
         <v>7</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>8</v>
+        <v>123</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B6" s="7"/>
     </row>
     <row r="7" spans="1:26" ht="216.75" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="5" t="s">
         <v>10</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="318.75" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="5" t="s">
         <v>12</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="409.5" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" s="6" t="s">
         <v>14</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="409.5" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" s="5" t="s">
         <v>16</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" s="5" t="s">
         <v>18</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="409.5" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12" s="5" t="s">
         <v>20</v>
-      </c>
-      <c r="B12" s="5" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="280.5" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13" s="5" t="s">
         <v>22</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="153" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B14" s="5" t="s">
         <v>24</v>
-      </c>
-      <c r="B14" s="5" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="409.5" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B15" s="5" t="s">
         <v>26</v>
-      </c>
-      <c r="B15" s="5" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B16" s="5" t="s">
         <v>28</v>
-      </c>
-      <c r="B16" s="5" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="B17" s="5" t="s">
         <v>118</v>
-      </c>
-      <c r="B17" s="5" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="51" x14ac:dyDescent="0.2">
       <c r="A20" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B20" s="9" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A21" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B21" s="7"/>
     </row>
     <row r="22" spans="1:2" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A22" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="B22" s="9" t="s">
         <v>33</v>
-      </c>
-      <c r="B22" s="9" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A23" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="B23" s="9" t="s">
         <v>35</v>
-      </c>
-      <c r="B23" s="9" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A24" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="B24" s="9" t="s">
         <v>37</v>
-      </c>
-      <c r="B24" s="9" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A25" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="B25" s="10" t="s">
         <v>39</v>
-      </c>
-      <c r="B25" s="10" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A26" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="B26" s="4" t="s">
         <v>41</v>
-      </c>
-      <c r="B26" s="4" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A27" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="B27" s="9" t="s">
         <v>43</v>
-      </c>
-      <c r="B27" s="9" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="28" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A28" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="B28" s="9" t="s">
         <v>45</v>
-      </c>
-      <c r="B28" s="9" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A29" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="B29" s="9" t="s">
         <v>47</v>
-      </c>
-      <c r="B29" s="9" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A30" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="B30" s="11" t="s">
         <v>49</v>
-      </c>
-      <c r="B30" s="11" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A31" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="B31" s="9" t="s">
         <v>51</v>
-      </c>
-      <c r="B31" s="9" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A32" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="B32" s="9" t="s">
         <v>53</v>
-      </c>
-      <c r="B32" s="9" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A33" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="B33" s="9" t="s">
         <v>55</v>
-      </c>
-      <c r="B33" s="9" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A34" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="B34" s="9" t="s">
         <v>57</v>
-      </c>
-      <c r="B34" s="9" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A35" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="B35" s="9" t="s">
         <v>59</v>
-      </c>
-      <c r="B35" s="9" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A36" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="B36" s="9" t="s">
         <v>61</v>
-      </c>
-      <c r="B36" s="9" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A37" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="B37" s="9" t="s">
         <v>63</v>
-      </c>
-      <c r="B37" s="9" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A38" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="B38" s="11" t="s">
         <v>65</v>
-      </c>
-      <c r="B38" s="11" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="39" spans="1:2" ht="153" x14ac:dyDescent="0.2">
       <c r="A39" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="B39" s="9" t="s">
         <v>67</v>
-      </c>
-      <c r="B39" s="9" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="40" spans="1:2" ht="140.25" x14ac:dyDescent="0.2">
       <c r="A40" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="B40" s="9" t="s">
         <v>69</v>
-      </c>
-      <c r="B40" s="9" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A41" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="B41" s="5" t="s">
         <v>71</v>
-      </c>
-      <c r="B41" s="5" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="42" spans="1:2" ht="395.25" x14ac:dyDescent="0.2">
       <c r="A42" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="B42" s="6" t="s">
         <v>73</v>
-      </c>
-      <c r="B42" s="6" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="43" spans="1:2" ht="331.5" x14ac:dyDescent="0.2">
       <c r="A43" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="B43" s="5" t="s">
         <v>75</v>
-      </c>
-      <c r="B43" s="5" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="44" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A44" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B44" s="5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="45" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A45" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="B45" s="6" t="s">
         <v>78</v>
-      </c>
-      <c r="B45" s="6" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="46" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A46" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B46" s="5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="47" spans="1:2" ht="51" x14ac:dyDescent="0.2">
       <c r="A47" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B47" s="5" t="s">
         <v>81</v>
-      </c>
-      <c r="B47" s="5" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="48" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A48" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="B48" s="5" t="s">
         <v>83</v>
-      </c>
-      <c r="B48" s="5" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="49" spans="1:2" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A49" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="B49" s="5" t="s">
         <v>85</v>
-      </c>
-      <c r="B49" s="5" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="50" spans="1:2" ht="306" x14ac:dyDescent="0.2">
       <c r="A50" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="B50" s="5" t="s">
         <v>87</v>
-      </c>
-      <c r="B50" s="5" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="51" spans="1:2" ht="63.75" x14ac:dyDescent="0.2">
       <c r="A51" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="B51" s="5" t="s">
         <v>89</v>
-      </c>
-      <c r="B51" s="5" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="52" spans="1:2" ht="51" x14ac:dyDescent="0.2">
       <c r="A52" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="B52" s="5" t="s">
         <v>91</v>
-      </c>
-      <c r="B52" s="5" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="53" spans="1:2" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="B53" s="6" t="s">
         <v>93</v>
-      </c>
-      <c r="B53" s="6" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="54" spans="1:2" ht="408" x14ac:dyDescent="0.2">
       <c r="A54" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="B54" s="6" t="s">
         <v>95</v>
-      </c>
-      <c r="B54" s="6" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="55" spans="1:2" ht="344.25" x14ac:dyDescent="0.2">
       <c r="A55" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="B55" s="5" t="s">
         <v>97</v>
-      </c>
-      <c r="B55" s="5" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="56" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A56" s="4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B56" s="7"/>
     </row>
     <row r="57" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A57" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B57" s="7"/>
     </row>
     <row r="58" spans="1:2" ht="51" x14ac:dyDescent="0.2">
       <c r="A58" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="B58" s="5" t="s">
         <v>101</v>
-      </c>
-      <c r="B58" s="5" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="59" spans="1:2" ht="51" x14ac:dyDescent="0.2">
       <c r="A59" s="4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B59" s="5" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="60" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A60" s="4" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B60" s="7"/>
     </row>
     <row r="61" spans="1:2" ht="51" x14ac:dyDescent="0.2">
       <c r="A61" s="4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B61" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="62" spans="1:2" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A62" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="B62" s="5" t="s">
         <v>106</v>
-      </c>
-      <c r="B62" s="5" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="63" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A63" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="B63" s="5" t="s">
         <v>108</v>
-      </c>
-      <c r="B63" s="5" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="64" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A64" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B64" s="7"/>
     </row>
     <row r="65" spans="1:2" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A65" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="B65" s="5" t="s">
         <v>111</v>
-      </c>
-      <c r="B65" s="5" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="66" spans="1:2" ht="216.75" x14ac:dyDescent="0.2">
       <c r="A66" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="B66" s="5" t="s">
         <v>113</v>
-      </c>
-      <c r="B66" s="5" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="67" spans="1:2" ht="178.5" x14ac:dyDescent="0.2">
       <c r="A67" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="B67" s="5" t="s">
         <v>115</v>
-      </c>
-      <c r="B67" s="5" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="68" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A68" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B68" s="7"/>
     </row>
@@ -4450,7 +4450,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B5" r:id="rId1" location="harf-A" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="B5" r:id="rId1" location="harf-A" display="Doğrudan bu https://kutuphane.itu.edu.tr/arastirma/veritabanlari#harf-A linkten veritabanlarına ulaşıp, bu veritabanları içerisinden Scopus veya Web of Science'a ulaşabilirsiniz. Ya da kütüphane anasayfasındaki &quot;Tarıyorum&quot; arama çubuğun hemen altındaki &quot;v" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
     <hyperlink ref="B9" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
     <hyperlink ref="B30" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
     <hyperlink ref="B38" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>

</xml_diff>